<commit_message>
Changed to Micro USB B.lbr
</commit_message>
<xml_diff>
--- a/V3.5/V3.5 BOM 20151209.xlsx
+++ b/V3.5/V3.5 BOM 20151209.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Li Nayu\Desktop\Course\iUROP\Eagle Design\V3.5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Li Nayu\Desktop\SENSg-V3.5\V3.5\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="228">
   <si>
     <t>Sub-System</t>
   </si>
@@ -773,7 +773,11 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>ALT SMD Micro USB</t>
+    <t>MICRO USB</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>MOLEX</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -1411,6 +1415,54 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="4" fillId="2" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="178" fontId="10" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1422,54 +1474,6 @@
     </xf>
     <xf numFmtId="178" fontId="7" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="7" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="7" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="2" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="7" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="7" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="7" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="7" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="7" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1760,7 +1764,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
@@ -1772,7 +1776,7 @@
     <col min="5" max="5" width="10.5" customWidth="1"/>
     <col min="6" max="6" width="16.8984375" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.59765625" customWidth="1"/>
-    <col min="8" max="8" width="9.69921875" customWidth="1"/>
+    <col min="8" max="8" width="20.8984375" customWidth="1"/>
     <col min="9" max="9" width="6" customWidth="1"/>
     <col min="10" max="10" width="12.09765625" customWidth="1"/>
     <col min="11" max="11" width="7.69921875" customWidth="1"/>
@@ -1818,7 +1822,7 @@
       <c r="N1" s="14"/>
     </row>
     <row r="2" spans="1:14" ht="21.75" customHeight="1">
-      <c r="A2" s="126" t="s">
+      <c r="A2" s="142" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="122" t="s">
@@ -1848,7 +1852,7 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="16.2">
-      <c r="A3" s="127"/>
+      <c r="A3" s="126"/>
       <c r="B3" s="112" t="s">
         <v>151</v>
       </c>
@@ -1882,7 +1886,7 @@
       <c r="N3" s="30"/>
     </row>
     <row r="4" spans="1:14" ht="16.2">
-      <c r="A4" s="127"/>
+      <c r="A4" s="126"/>
       <c r="B4" s="109" t="s">
         <v>8</v>
       </c>
@@ -1916,15 +1920,15 @@
       <c r="N4" s="30"/>
     </row>
     <row r="5" spans="1:14" ht="16.2">
-      <c r="A5" s="127"/>
-      <c r="B5" s="112" t="s">
+      <c r="A5" s="126"/>
+      <c r="B5" s="121" t="s">
         <v>226</v>
       </c>
       <c r="C5" s="20" t="s">
         <v>108</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>143</v>
+        <v>227</v>
       </c>
       <c r="E5" s="31" t="s">
         <v>109</v>
@@ -1934,7 +1938,7 @@
         <v>7</v>
       </c>
       <c r="H5" s="24">
-        <v>2293752</v>
+        <v>1568026</v>
       </c>
       <c r="I5" s="28">
         <v>1</v>
@@ -1948,7 +1952,7 @@
       <c r="N5" s="35"/>
     </row>
     <row r="6" spans="1:14" ht="16.2">
-      <c r="A6" s="127"/>
+      <c r="A6" s="126"/>
       <c r="B6" s="110" t="s">
         <v>9</v>
       </c>
@@ -1982,7 +1986,7 @@
       <c r="N6" s="30"/>
     </row>
     <row r="7" spans="1:14" ht="16.2">
-      <c r="A7" s="127"/>
+      <c r="A7" s="126"/>
       <c r="B7" s="109" t="s">
         <v>10</v>
       </c>
@@ -2016,7 +2020,7 @@
       <c r="N7" s="30"/>
     </row>
     <row r="8" spans="1:14" ht="16.2">
-      <c r="A8" s="127"/>
+      <c r="A8" s="126"/>
       <c r="B8" s="110" t="s">
         <v>11</v>
       </c>
@@ -2050,7 +2054,7 @@
       <c r="N8" s="30"/>
     </row>
     <row r="9" spans="1:14" ht="16.2">
-      <c r="A9" s="127"/>
+      <c r="A9" s="126"/>
       <c r="B9" s="109" t="s">
         <v>12</v>
       </c>
@@ -2084,7 +2088,7 @@
       <c r="N9" s="30"/>
     </row>
     <row r="10" spans="1:14" ht="16.2">
-      <c r="A10" s="127"/>
+      <c r="A10" s="126"/>
       <c r="B10" s="111" t="s">
         <v>14</v>
       </c>
@@ -2118,7 +2122,7 @@
       <c r="N10" s="30"/>
     </row>
     <row r="11" spans="1:14" ht="16.2">
-      <c r="A11" s="127"/>
+      <c r="A11" s="126"/>
       <c r="B11" s="112" t="s">
         <v>132</v>
       </c>
@@ -2150,7 +2154,7 @@
       <c r="N11" s="30"/>
     </row>
     <row r="12" spans="1:14" ht="16.2">
-      <c r="A12" s="127"/>
+      <c r="A12" s="126"/>
       <c r="B12" s="110" t="s">
         <v>35</v>
       </c>
@@ -2184,7 +2188,7 @@
       <c r="N12" s="30"/>
     </row>
     <row r="13" spans="1:14" ht="16.2">
-      <c r="A13" s="127"/>
+      <c r="A13" s="126"/>
       <c r="B13" s="109" t="s">
         <v>13</v>
       </c>
@@ -2216,7 +2220,7 @@
       <c r="N13" s="30"/>
     </row>
     <row r="14" spans="1:14" ht="16.2">
-      <c r="A14" s="128"/>
+      <c r="A14" s="127"/>
       <c r="B14" s="117" t="s">
         <v>124</v>
       </c>
@@ -2250,7 +2254,7 @@
       <c r="N14" s="48"/>
     </row>
     <row r="15" spans="1:14" ht="16.2">
-      <c r="A15" s="127" t="s">
+      <c r="A15" s="126" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="113" t="s">
@@ -2284,7 +2288,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" ht="16.2">
-      <c r="A16" s="127"/>
+      <c r="A16" s="126"/>
       <c r="B16" s="111" t="s">
         <v>14</v>
       </c>
@@ -2318,7 +2322,7 @@
       <c r="N16" s="30"/>
     </row>
     <row r="17" spans="1:14" ht="16.2">
-      <c r="A17" s="127"/>
+      <c r="A17" s="126"/>
       <c r="B17" s="114" t="s">
         <v>134</v>
       </c>
@@ -2352,7 +2356,7 @@
       <c r="N17" s="30"/>
     </row>
     <row r="18" spans="1:14" ht="16.2">
-      <c r="A18" s="127"/>
+      <c r="A18" s="126"/>
       <c r="B18" s="110" t="s">
         <v>20</v>
       </c>
@@ -2386,7 +2390,7 @@
       <c r="N18" s="55"/>
     </row>
     <row r="19" spans="1:14" ht="31.2">
-      <c r="A19" s="127"/>
+      <c r="A19" s="126"/>
       <c r="B19" s="111" t="s">
         <v>58</v>
       </c>
@@ -2420,7 +2424,7 @@
       <c r="N19" s="55"/>
     </row>
     <row r="20" spans="1:14" ht="16.2">
-      <c r="A20" s="127"/>
+      <c r="A20" s="126"/>
       <c r="B20" s="114" t="s">
         <v>148</v>
       </c>
@@ -2454,7 +2458,7 @@
       <c r="N20" s="55"/>
     </row>
     <row r="21" spans="1:14" ht="16.2">
-      <c r="A21" s="127"/>
+      <c r="A21" s="126"/>
       <c r="B21" s="111" t="s">
         <v>22</v>
       </c>
@@ -2486,7 +2490,7 @@
       <c r="N21" s="55"/>
     </row>
     <row r="22" spans="1:14" ht="16.2">
-      <c r="A22" s="127"/>
+      <c r="A22" s="126"/>
       <c r="B22" s="110" t="s">
         <v>23</v>
       </c>
@@ -2520,7 +2524,7 @@
       <c r="N22" s="55"/>
     </row>
     <row r="23" spans="1:14" ht="16.2">
-      <c r="A23" s="127"/>
+      <c r="A23" s="126"/>
       <c r="B23" s="121" t="s">
         <v>24</v>
       </c>
@@ -2552,7 +2556,7 @@
       <c r="N23" s="55"/>
     </row>
     <row r="24" spans="1:14" ht="16.2">
-      <c r="A24" s="127"/>
+      <c r="A24" s="126"/>
       <c r="B24" s="115" t="s">
         <v>25</v>
       </c>
@@ -2584,7 +2588,7 @@
       <c r="N24" s="55"/>
     </row>
     <row r="25" spans="1:14" ht="16.2">
-      <c r="A25" s="127"/>
+      <c r="A25" s="126"/>
       <c r="B25" s="110" t="s">
         <v>54</v>
       </c>
@@ -2618,7 +2622,7 @@
       <c r="N25" s="55"/>
     </row>
     <row r="26" spans="1:14" ht="16.2">
-      <c r="A26" s="127"/>
+      <c r="A26" s="126"/>
       <c r="B26" s="115" t="s">
         <v>62</v>
       </c>
@@ -2652,7 +2656,7 @@
       <c r="N26" s="55"/>
     </row>
     <row r="27" spans="1:14" ht="16.2">
-      <c r="A27" s="127"/>
+      <c r="A27" s="126"/>
       <c r="B27" s="115" t="s">
         <v>55</v>
       </c>
@@ -2686,7 +2690,7 @@
       <c r="N27" s="55"/>
     </row>
     <row r="28" spans="1:14" ht="16.2">
-      <c r="A28" s="127"/>
+      <c r="A28" s="126"/>
       <c r="B28" s="116" t="s">
         <v>128</v>
       </c>
@@ -2720,7 +2724,7 @@
       <c r="N28" s="55"/>
     </row>
     <row r="29" spans="1:14" ht="16.2">
-      <c r="A29" s="123" t="s">
+      <c r="A29" s="139" t="s">
         <v>26</v>
       </c>
       <c r="B29" s="111" t="s">
@@ -2748,7 +2752,7 @@
       <c r="N29" s="64"/>
     </row>
     <row r="30" spans="1:14" ht="16.2">
-      <c r="A30" s="124"/>
+      <c r="A30" s="140"/>
       <c r="B30" s="65" t="s">
         <v>63</v>
       </c>
@@ -2776,7 +2780,7 @@
       <c r="N30" s="48"/>
     </row>
     <row r="31" spans="1:14" ht="16.2">
-      <c r="A31" s="123" t="s">
+      <c r="A31" s="139" t="s">
         <v>28</v>
       </c>
       <c r="B31" s="113" t="s">
@@ -2808,7 +2812,7 @@
       <c r="N31" s="30"/>
     </row>
     <row r="32" spans="1:14" ht="16.2">
-      <c r="A32" s="124"/>
+      <c r="A32" s="140"/>
       <c r="B32" s="111" t="s">
         <v>14</v>
       </c>
@@ -2842,7 +2846,7 @@
       <c r="N32" s="30"/>
     </row>
     <row r="33" spans="1:14" ht="16.2">
-      <c r="A33" s="124"/>
+      <c r="A33" s="140"/>
       <c r="B33" s="114" t="s">
         <v>29</v>
       </c>
@@ -2874,7 +2878,7 @@
       <c r="N33" s="30"/>
     </row>
     <row r="34" spans="1:14" ht="16.2">
-      <c r="A34" s="124"/>
+      <c r="A34" s="140"/>
       <c r="B34" s="111" t="s">
         <v>30</v>
       </c>
@@ -2908,7 +2912,7 @@
       <c r="N34" s="30"/>
     </row>
     <row r="35" spans="1:14" ht="16.2">
-      <c r="A35" s="125"/>
+      <c r="A35" s="141"/>
       <c r="B35" s="75"/>
       <c r="C35" s="76"/>
       <c r="D35" s="76"/>
@@ -2924,7 +2928,7 @@
       <c r="N35" s="48"/>
     </row>
     <row r="36" spans="1:14" ht="31.2">
-      <c r="A36" s="123" t="s">
+      <c r="A36" s="139" t="s">
         <v>31</v>
       </c>
       <c r="B36" s="119" t="s">
@@ -2956,7 +2960,7 @@
       <c r="N36" s="30"/>
     </row>
     <row r="37" spans="1:14" ht="16.2">
-      <c r="A37" s="124"/>
+      <c r="A37" s="140"/>
       <c r="B37" s="121" t="s">
         <v>218</v>
       </c>
@@ -2990,7 +2994,7 @@
       <c r="N37" s="30"/>
     </row>
     <row r="38" spans="1:14" ht="16.2">
-      <c r="A38" s="125"/>
+      <c r="A38" s="141"/>
       <c r="B38" s="116" t="s">
         <v>217</v>
       </c>
@@ -3024,7 +3028,7 @@
       <c r="N38" s="30"/>
     </row>
     <row r="39" spans="1:14" ht="16.2">
-      <c r="A39" s="131" t="s">
+      <c r="A39" s="125" t="s">
         <v>32</v>
       </c>
       <c r="B39" s="120" t="s">
@@ -3060,7 +3064,7 @@
       <c r="N39" s="54"/>
     </row>
     <row r="40" spans="1:14" ht="16.2">
-      <c r="A40" s="127"/>
+      <c r="A40" s="126"/>
       <c r="B40" s="111" t="s">
         <v>34</v>
       </c>
@@ -3094,7 +3098,7 @@
       <c r="N40" s="30"/>
     </row>
     <row r="41" spans="1:14" ht="16.2">
-      <c r="A41" s="127"/>
+      <c r="A41" s="126"/>
       <c r="B41" s="110" t="s">
         <v>20</v>
       </c>
@@ -3128,7 +3132,7 @@
       <c r="N41" s="30"/>
     </row>
     <row r="42" spans="1:14" ht="16.2">
-      <c r="A42" s="127"/>
+      <c r="A42" s="126"/>
       <c r="B42" s="114" t="s">
         <v>137</v>
       </c>
@@ -3162,7 +3166,7 @@
       <c r="N42" s="30"/>
     </row>
     <row r="43" spans="1:14" ht="16.2">
-      <c r="A43" s="127"/>
+      <c r="A43" s="126"/>
       <c r="B43" s="111" t="s">
         <v>135</v>
       </c>
@@ -3196,7 +3200,7 @@
       <c r="N43" s="30"/>
     </row>
     <row r="44" spans="1:14" ht="16.2">
-      <c r="A44" s="127"/>
+      <c r="A44" s="126"/>
       <c r="B44" s="114" t="s">
         <v>149</v>
       </c>
@@ -3230,7 +3234,7 @@
       <c r="N44" s="30"/>
     </row>
     <row r="45" spans="1:14" ht="16.2">
-      <c r="A45" s="127"/>
+      <c r="A45" s="126"/>
       <c r="B45" s="111" t="s">
         <v>9</v>
       </c>
@@ -3264,7 +3268,7 @@
       <c r="N45" s="30"/>
     </row>
     <row r="46" spans="1:14" ht="16.2">
-      <c r="A46" s="127"/>
+      <c r="A46" s="126"/>
       <c r="B46" s="121" t="s">
         <v>36</v>
       </c>
@@ -3298,7 +3302,7 @@
       <c r="N46" s="30"/>
     </row>
     <row r="47" spans="1:14" ht="16.2">
-      <c r="A47" s="128"/>
+      <c r="A47" s="127"/>
       <c r="B47" s="111" t="s">
         <v>14</v>
       </c>
@@ -3332,7 +3336,7 @@
       <c r="N47" s="52"/>
     </row>
     <row r="48" spans="1:14" ht="16.2">
-      <c r="A48" s="132" t="s">
+      <c r="A48" s="128" t="s">
         <v>38</v>
       </c>
       <c r="B48" s="118" t="s">
@@ -3362,7 +3366,7 @@
       <c r="N48" s="64"/>
     </row>
     <row r="49" spans="1:14" ht="16.2">
-      <c r="A49" s="133"/>
+      <c r="A49" s="129"/>
       <c r="B49" s="111" t="s">
         <v>14</v>
       </c>
@@ -3396,7 +3400,7 @@
       <c r="N49" s="48"/>
     </row>
     <row r="50" spans="1:14" ht="16.2">
-      <c r="A50" s="131" t="s">
+      <c r="A50" s="125" t="s">
         <v>40</v>
       </c>
       <c r="B50" s="118" t="s">
@@ -3428,7 +3432,7 @@
       <c r="N50" s="86"/>
     </row>
     <row r="51" spans="1:14" ht="16.2">
-      <c r="A51" s="127"/>
+      <c r="A51" s="126"/>
       <c r="B51" s="111" t="s">
         <v>43</v>
       </c>
@@ -3462,7 +3466,7 @@
       <c r="N51" s="87"/>
     </row>
     <row r="52" spans="1:14" ht="16.2">
-      <c r="A52" s="127"/>
+      <c r="A52" s="126"/>
       <c r="B52" s="111" t="s">
         <v>14</v>
       </c>
@@ -3496,7 +3500,7 @@
       <c r="N52" s="88"/>
     </row>
     <row r="53" spans="1:14" ht="16.2">
-      <c r="A53" s="134"/>
+      <c r="A53" s="130"/>
       <c r="B53" s="59"/>
       <c r="C53" s="40"/>
       <c r="D53" s="41"/>
@@ -3512,7 +3516,7 @@
       <c r="N53" s="89"/>
     </row>
     <row r="54" spans="1:14" ht="16.2">
-      <c r="A54" s="131" t="s">
+      <c r="A54" s="125" t="s">
         <v>44</v>
       </c>
       <c r="B54" s="111" t="s">
@@ -3546,7 +3550,7 @@
       <c r="N54" s="90"/>
     </row>
     <row r="55" spans="1:14" ht="16.2">
-      <c r="A55" s="127"/>
+      <c r="A55" s="126"/>
       <c r="B55" s="111" t="s">
         <v>20</v>
       </c>
@@ -3580,7 +3584,7 @@
       <c r="N55" s="88"/>
     </row>
     <row r="56" spans="1:14" ht="16.2">
-      <c r="A56" s="127"/>
+      <c r="A56" s="126"/>
       <c r="B56" s="111" t="s">
         <v>14</v>
       </c>
@@ -3614,7 +3618,7 @@
       <c r="N56" s="88"/>
     </row>
     <row r="57" spans="1:14" ht="16.2">
-      <c r="A57" s="127"/>
+      <c r="A57" s="126"/>
       <c r="B57" s="49"/>
       <c r="C57" s="20"/>
       <c r="D57" s="31"/>
@@ -3630,7 +3634,7 @@
       <c r="N57" s="88"/>
     </row>
     <row r="58" spans="1:14" ht="16.2">
-      <c r="A58" s="128"/>
+      <c r="A58" s="127"/>
       <c r="B58" s="59"/>
       <c r="C58" s="40"/>
       <c r="D58" s="41"/>
@@ -3646,7 +3650,7 @@
       <c r="N58" s="91"/>
     </row>
     <row r="59" spans="1:14" ht="16.2">
-      <c r="A59" s="132" t="s">
+      <c r="A59" s="128" t="s">
         <v>47</v>
       </c>
       <c r="B59" s="113" t="s">
@@ -3682,7 +3686,7 @@
       </c>
     </row>
     <row r="60" spans="1:14" ht="16.2">
-      <c r="A60" s="133"/>
+      <c r="A60" s="129"/>
       <c r="B60" s="59"/>
       <c r="C60" s="40"/>
       <c r="D60" s="94"/>
@@ -3698,7 +3702,7 @@
       <c r="N60" s="96"/>
     </row>
     <row r="61" spans="1:14" ht="16.2">
-      <c r="A61" s="132" t="s">
+      <c r="A61" s="128" t="s">
         <v>49</v>
       </c>
       <c r="B61" s="68" t="s">
@@ -3732,7 +3736,7 @@
       </c>
     </row>
     <row r="62" spans="1:14" ht="16.2">
-      <c r="A62" s="135"/>
+      <c r="A62" s="131"/>
       <c r="B62" s="53" t="s">
         <v>220</v>
       </c>
@@ -3766,7 +3770,7 @@
       <c r="N62" s="30"/>
     </row>
     <row r="63" spans="1:14" ht="16.2">
-      <c r="A63" s="133"/>
+      <c r="A63" s="129"/>
       <c r="B63" s="116" t="s">
         <v>139</v>
       </c>
@@ -3796,7 +3800,7 @@
       <c r="N63" s="89"/>
     </row>
     <row r="64" spans="1:14" ht="16.2">
-      <c r="A64" s="131" t="s">
+      <c r="A64" s="125" t="s">
         <v>50</v>
       </c>
       <c r="B64" s="97" t="s">
@@ -3818,7 +3822,7 @@
       <c r="N64" s="64"/>
     </row>
     <row r="65" spans="1:14" ht="16.2">
-      <c r="A65" s="127"/>
+      <c r="A65" s="126"/>
       <c r="B65" s="100"/>
       <c r="C65" s="101"/>
       <c r="D65" s="31"/>
@@ -3834,7 +3838,7 @@
       <c r="N65" s="30"/>
     </row>
     <row r="66" spans="1:14" ht="16.2">
-      <c r="A66" s="127"/>
+      <c r="A66" s="126"/>
       <c r="B66" s="100"/>
       <c r="C66" s="101"/>
       <c r="D66" s="31"/>
@@ -3850,7 +3854,7 @@
       <c r="N66" s="30"/>
     </row>
     <row r="67" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A67" s="128"/>
+      <c r="A67" s="127"/>
       <c r="B67" s="59"/>
       <c r="C67" s="40"/>
       <c r="D67" s="41"/>
@@ -3866,7 +3870,7 @@
       <c r="N67" s="48"/>
     </row>
     <row r="68" spans="1:14" ht="16.2">
-      <c r="A68" s="131" t="s">
+      <c r="A68" s="125" t="s">
         <v>51</v>
       </c>
       <c r="B68" s="120" t="s">
@@ -3900,7 +3904,7 @@
       <c r="N68" s="64"/>
     </row>
     <row r="69" spans="1:14" ht="16.2">
-      <c r="A69" s="127"/>
+      <c r="A69" s="126"/>
       <c r="B69" s="49"/>
       <c r="C69" s="20"/>
       <c r="D69" s="31"/>
@@ -3916,7 +3920,7 @@
       <c r="N69" s="55"/>
     </row>
     <row r="70" spans="1:14" ht="16.2">
-      <c r="A70" s="127"/>
+      <c r="A70" s="126"/>
       <c r="B70" s="49"/>
       <c r="C70" s="20"/>
       <c r="D70" s="31"/>
@@ -3932,7 +3936,7 @@
       <c r="N70" s="55"/>
     </row>
     <row r="71" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A71" s="128"/>
+      <c r="A71" s="127"/>
       <c r="B71" s="59"/>
       <c r="C71" s="40"/>
       <c r="D71" s="41"/>
@@ -3949,38 +3953,43 @@
     </row>
     <row r="72" spans="1:14" ht="16.2" thickBot="1"/>
     <row r="73" spans="1:14" ht="32.25" customHeight="1" thickTop="1">
-      <c r="A73" s="136"/>
+      <c r="A73" s="132"/>
       <c r="B73" s="11"/>
       <c r="C73" s="11"/>
       <c r="D73" s="3"/>
       <c r="E73" s="3"/>
-      <c r="F73" s="138"/>
-      <c r="G73" s="139"/>
-      <c r="H73" s="139"/>
-      <c r="I73" s="141"/>
+      <c r="F73" s="134"/>
+      <c r="G73" s="135"/>
+      <c r="H73" s="135"/>
+      <c r="I73" s="137"/>
       <c r="J73" s="4"/>
       <c r="K73" s="5"/>
       <c r="L73" s="6"/>
-      <c r="M73" s="129"/>
+      <c r="M73" s="123"/>
     </row>
     <row r="74" spans="1:14">
-      <c r="A74" s="137"/>
+      <c r="A74" s="133"/>
       <c r="B74" s="12"/>
       <c r="C74" s="12"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
-      <c r="F74" s="140"/>
-      <c r="G74" s="140"/>
-      <c r="H74" s="140"/>
-      <c r="I74" s="142"/>
+      <c r="F74" s="136"/>
+      <c r="G74" s="136"/>
+      <c r="H74" s="136"/>
+      <c r="I74" s="138"/>
       <c r="J74" s="7"/>
       <c r="K74" s="8"/>
       <c r="L74" s="8"/>
-      <c r="M74" s="130"/>
+      <c r="M74" s="124"/>
       <c r="N74" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="A2:A14"/>
+    <mergeCell ref="A15:A28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A31:A35"/>
     <mergeCell ref="M73:M74"/>
     <mergeCell ref="A39:A47"/>
     <mergeCell ref="A48:A49"/>
@@ -3993,11 +4002,6 @@
     <mergeCell ref="A73:A74"/>
     <mergeCell ref="F73:H74"/>
     <mergeCell ref="I73:I74"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="A2:A14"/>
-    <mergeCell ref="A15:A28"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A31:A35"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
@@ -4037,31 +4041,31 @@
     <hyperlink ref="B3" r:id="rId34" display="3.3v LDO"/>
     <hyperlink ref="B24" r:id="rId35"/>
     <hyperlink ref="B25" r:id="rId36"/>
-    <hyperlink ref="B5" r:id="rId37"/>
-    <hyperlink ref="B27" r:id="rId38"/>
-    <hyperlink ref="B30" r:id="rId39"/>
-    <hyperlink ref="B31" r:id="rId40"/>
-    <hyperlink ref="G31" r:id="rId41"/>
-    <hyperlink ref="B59" r:id="rId42" display="14mm DIA Buzzer"/>
-    <hyperlink ref="B61" r:id="rId43"/>
-    <hyperlink ref="B26" r:id="rId44"/>
-    <hyperlink ref="B14" r:id="rId45"/>
-    <hyperlink ref="D14" r:id="rId46" display="http://www.mouser.sg/Taiyo-Yuden/"/>
-    <hyperlink ref="B28" r:id="rId47"/>
-    <hyperlink ref="B42" r:id="rId48"/>
-    <hyperlink ref="B10" r:id="rId49"/>
-    <hyperlink ref="B18" r:id="rId50" display="10K OHM"/>
-    <hyperlink ref="B16" r:id="rId51"/>
-    <hyperlink ref="B17" r:id="rId52"/>
-    <hyperlink ref="B11" r:id="rId53"/>
-    <hyperlink ref="B63" r:id="rId54"/>
-    <hyperlink ref="B68" r:id="rId55"/>
-    <hyperlink ref="D39" r:id="rId56" display="http://sg.element14.com/projects-unlimited"/>
-    <hyperlink ref="B20" r:id="rId57"/>
-    <hyperlink ref="B44" r:id="rId58"/>
-    <hyperlink ref="B37" r:id="rId59" display="1K OHM 1%"/>
-    <hyperlink ref="B38" r:id="rId60"/>
-    <hyperlink ref="B62" r:id="rId61"/>
+    <hyperlink ref="B27" r:id="rId37"/>
+    <hyperlink ref="B30" r:id="rId38"/>
+    <hyperlink ref="B31" r:id="rId39"/>
+    <hyperlink ref="G31" r:id="rId40"/>
+    <hyperlink ref="B59" r:id="rId41" display="14mm DIA Buzzer"/>
+    <hyperlink ref="B61" r:id="rId42"/>
+    <hyperlink ref="B26" r:id="rId43"/>
+    <hyperlink ref="B14" r:id="rId44"/>
+    <hyperlink ref="D14" r:id="rId45" display="http://www.mouser.sg/Taiyo-Yuden/"/>
+    <hyperlink ref="B28" r:id="rId46"/>
+    <hyperlink ref="B42" r:id="rId47"/>
+    <hyperlink ref="B10" r:id="rId48"/>
+    <hyperlink ref="B18" r:id="rId49" display="10K OHM"/>
+    <hyperlink ref="B16" r:id="rId50"/>
+    <hyperlink ref="B17" r:id="rId51"/>
+    <hyperlink ref="B11" r:id="rId52"/>
+    <hyperlink ref="B63" r:id="rId53"/>
+    <hyperlink ref="B68" r:id="rId54"/>
+    <hyperlink ref="D39" r:id="rId55" display="http://sg.element14.com/projects-unlimited"/>
+    <hyperlink ref="B20" r:id="rId56"/>
+    <hyperlink ref="B44" r:id="rId57"/>
+    <hyperlink ref="B37" r:id="rId58" display="1K OHM 1%"/>
+    <hyperlink ref="B38" r:id="rId59"/>
+    <hyperlink ref="B62" r:id="rId60"/>
+    <hyperlink ref="B5" r:id="rId61"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="44" orientation="portrait" r:id="rId62"/>

</xml_diff>